<commit_message>
Modify report - add chart
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="367">
   <si>
     <t>Description</t>
   </si>
@@ -1131,12 +1131,6 @@
   </si>
   <si>
     <t>Demo</t>
-  </si>
-  <si>
-    <t>TC_DN2</t>
-  </si>
-  <si>
-    <t>TC_DN4</t>
   </si>
   <si>
     <t>TC_DN1</t>
@@ -2969,10 +2963,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3007,7 +3001,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>362</v>
@@ -3022,44 +3016,9 @@
         <v>365</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>366</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>367</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>58</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" display="hoanganh04092001@gmail.com"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
update data for Excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Keywords" sheetId="3" state="hidden" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="SignUpPageOriginal" sheetId="2" state="hidden" r:id="rId5"/>
     <sheet name="SignUpPage" sheetId="10" r:id="rId6"/>
     <sheet name="DataOfSignUp" sheetId="5" r:id="rId7"/>
-    <sheet name="CreateCV" sheetId="6" state="hidden" r:id="rId8"/>
+    <sheet name="CreateCV" sheetId="6" r:id="rId8"/>
     <sheet name="DataOfCreateCV" sheetId="7" state="hidden" r:id="rId9"/>
     <sheet name="Search" sheetId="8" state="hidden" r:id="rId10"/>
   </sheets>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1031" uniqueCount="370">
   <si>
     <t>Description</t>
   </si>
@@ -806,9 +806,6 @@
     <t>TSCV11</t>
   </si>
   <si>
-    <t>TSCV11_DN</t>
-  </si>
-  <si>
     <t>TSCV11_CreateCV</t>
   </si>
   <si>
@@ -1082,9 +1079,6 @@
     <t>StepID</t>
   </si>
   <si>
-    <t>SSI_01</t>
-  </si>
-  <si>
     <t>S_01</t>
   </si>
   <si>
@@ -1134,6 +1128,21 @@
   </si>
   <si>
     <t>getURL</t>
+  </si>
+  <si>
+    <t>TC_DN2</t>
+  </si>
+  <si>
+    <t>LoginWithoutEmail</t>
+  </si>
+  <si>
+    <t>LoginWithoutPassword</t>
+  </si>
+  <si>
+    <t>Validate data in Email field</t>
+  </si>
+  <si>
+    <t>Validate data in Password field</t>
   </si>
 </sst>
 </file>
@@ -2073,7 +2082,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2081,7 +2090,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2185,7 +2194,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -2193,7 +2202,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -2201,7 +2210,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -2209,7 +2218,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -2217,7 +2226,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -2308,11 +2317,11 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B2" s="27"/>
       <c r="C2" s="28" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>6</v>
@@ -2347,7 +2356,7 @@
         <v>8</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2355,7 +2364,7 @@
       <c r="B4" s="24"/>
       <c r="C4" s="3"/>
       <c r="D4" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
@@ -2364,10 +2373,10 @@
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -2375,7 +2384,7 @@
       <c r="B5" s="24"/>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -2384,7 +2393,7 @@
         <v>20</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="H5" s="18"/>
     </row>
@@ -2393,7 +2402,7 @@
       <c r="B6" s="24"/>
       <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>33</v>
@@ -2402,7 +2411,7 @@
         <v>20</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>249</v>
@@ -2413,7 +2422,7 @@
       <c r="B7" s="24"/>
       <c r="C7" s="3"/>
       <c r="D7" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>33</v>
@@ -2422,10 +2431,10 @@
         <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>311</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -2433,7 +2442,7 @@
       <c r="B8" s="24"/>
       <c r="C8" s="3"/>
       <c r="D8" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>67</v>
@@ -2442,13 +2451,13 @@
         <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="3"/>
@@ -2470,12 +2479,12 @@
         <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2483,7 +2492,7 @@
       <c r="B11" s="64"/>
       <c r="C11" s="65"/>
       <c r="D11" s="66" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E11" s="66" t="s">
         <v>19</v>
@@ -2492,7 +2501,7 @@
         <v>20</v>
       </c>
       <c r="G11" s="68" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H11" s="67"/>
     </row>
@@ -2501,15 +2510,15 @@
       <c r="B12" s="64"/>
       <c r="C12" s="65"/>
       <c r="D12" s="66" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E12" s="66" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="F12" s="66"/>
       <c r="G12" s="66"/>
       <c r="H12" s="67" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2517,7 +2526,7 @@
       <c r="B13" s="64"/>
       <c r="C13" s="65"/>
       <c r="D13" s="66" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E13" s="66" t="s">
         <v>37</v>
@@ -2526,10 +2535,10 @@
         <v>20</v>
       </c>
       <c r="G13" s="66" t="s">
+        <v>330</v>
+      </c>
+      <c r="H13" s="67" t="s">
         <v>331</v>
-      </c>
-      <c r="H13" s="67" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2537,7 +2546,7 @@
       <c r="B14" s="64"/>
       <c r="C14" s="65"/>
       <c r="D14" s="66" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E14" s="66" t="s">
         <v>37</v>
@@ -2546,10 +2555,10 @@
         <v>20</v>
       </c>
       <c r="G14" s="66" t="s">
+        <v>322</v>
+      </c>
+      <c r="H14" s="69" t="s">
         <v>323</v>
-      </c>
-      <c r="H14" s="69" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -2557,7 +2566,7 @@
       <c r="B15" s="64"/>
       <c r="C15" s="65"/>
       <c r="D15" s="66" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>37</v>
@@ -2566,10 +2575,10 @@
         <v>20</v>
       </c>
       <c r="G15" s="66" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="H15" s="67" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -2577,7 +2586,7 @@
       <c r="B16" s="64"/>
       <c r="C16" s="65"/>
       <c r="D16" s="66" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>37</v>
@@ -2586,15 +2595,15 @@
         <v>20</v>
       </c>
       <c r="G16" s="66" t="s">
+        <v>328</v>
+      </c>
+      <c r="H16" s="67" t="s">
         <v>329</v>
-      </c>
-      <c r="H16" s="67" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B17" s="64"/>
       <c r="C17" s="65"/>
@@ -2664,7 +2673,7 @@
         <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2746,34 +2755,34 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="76" customWidth="1"/>
+    <col min="1" max="1" width="20" style="76" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.21875" style="76" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="76" customWidth="1"/>
     <col min="4" max="4" width="30.33203125" style="74" customWidth="1"/>
-    <col min="5" max="5" width="31.44140625" style="74" customWidth="1"/>
+    <col min="5" max="5" width="25.5546875" style="74" customWidth="1"/>
     <col min="6" max="6" width="16.44140625" style="74" customWidth="1"/>
-    <col min="7" max="7" width="40.77734375" style="74" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" style="74" customWidth="1"/>
     <col min="8" max="8" width="49.77734375" style="74" customWidth="1"/>
     <col min="9" max="16384" width="8.88671875" style="74"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
+        <v>345</v>
+      </c>
+      <c r="B1" s="77" t="s">
         <v>346</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="C1" s="77" t="s">
         <v>347</v>
-      </c>
-      <c r="C1" s="77" t="s">
-        <v>348</v>
       </c>
       <c r="D1" s="77" t="s">
         <v>0</v>
@@ -2782,24 +2791,24 @@
         <v>26</v>
       </c>
       <c r="F1" s="77" t="s">
+        <v>339</v>
+      </c>
+      <c r="G1" s="77" t="s">
         <v>340</v>
       </c>
-      <c r="G1" s="77" t="s">
-        <v>341</v>
-      </c>
       <c r="H1" s="77" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="75" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="71" t="s">
-        <v>349</v>
+        <v>366</v>
       </c>
       <c r="B2" s="78" t="s">
-        <v>345</v>
+        <v>368</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D2" s="72" t="s">
         <v>6</v>
@@ -2818,10 +2827,12 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
+      <c r="A3" s="71" t="s">
+        <v>366</v>
+      </c>
       <c r="B3" s="3"/>
       <c r="C3" s="71" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>64</v>
@@ -2840,10 +2851,12 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="71" t="s">
+        <v>366</v>
+      </c>
       <c r="B4" s="3"/>
       <c r="C4" s="71" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
@@ -2857,15 +2870,15 @@
       <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="71" t="s">
+        <v>366</v>
+      </c>
       <c r="B5" s="3"/>
       <c r="C5" s="71" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>65</v>
@@ -2879,15 +2892,17 @@
       <c r="G5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="79" t="s">
-        <v>53</v>
+      <c r="H5" s="79">
+        <v>20102001</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+      <c r="A6" s="71" t="s">
+        <v>366</v>
+      </c>
       <c r="B6" s="3"/>
       <c r="C6" s="71" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>66</v>
@@ -2904,28 +2919,32 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
+      <c r="A7" s="71" t="s">
+        <v>366</v>
+      </c>
       <c r="B7" s="3"/>
       <c r="C7" s="71" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>54</v>
+        <v>361</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
+      <c r="A8" s="71" t="s">
+        <v>366</v>
+      </c>
       <c r="B8" s="3"/>
       <c r="C8" s="71" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>23</v>
@@ -2936,6 +2955,162 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="71" t="s">
+        <v>367</v>
+      </c>
+      <c r="B9" s="78" t="s">
+        <v>369</v>
+      </c>
+      <c r="C9" s="71" t="s">
+        <v>348</v>
+      </c>
+      <c r="D9" s="72" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="72" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="72" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="71" t="s">
+        <v>367</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="71" t="s">
+        <v>349</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="71" t="s">
+        <v>367</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="71" t="s">
+        <v>350</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="71" t="s">
+        <v>367</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="71" t="s">
+        <v>351</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="79"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="71" t="s">
+        <v>367</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="71" t="s">
+        <v>352</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="71" t="s">
+        <v>367</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="71" t="s">
+        <v>353</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="37" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="71" t="s">
+        <v>367</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="71" t="s">
+        <v>354</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2963,10 +3138,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1"/>
+    <sheetView zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2984,7 +3159,7 @@
         <v>42</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C1" s="32" t="s">
         <v>38</v>
@@ -3001,19 +3176,33 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>362</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>363</v>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>358</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -3042,7 +3231,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>113</v>
@@ -4251,13 +4440,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
+        <v>345</v>
+      </c>
+      <c r="B1" s="77" t="s">
         <v>346</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="C1" s="77" t="s">
         <v>347</v>
-      </c>
-      <c r="C1" s="77" t="s">
-        <v>348</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>0</v>
@@ -4266,24 +4455,24 @@
         <v>26</v>
       </c>
       <c r="F1" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>340</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>341</v>
-      </c>
       <c r="H1" s="15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="70" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B2" s="78" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D2" s="72" t="s">
         <v>6</v>
@@ -4305,7 +4494,7 @@
       <c r="A3" s="16"/>
       <c r="B3" s="24"/>
       <c r="C3" s="71" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>64</v>
@@ -4327,7 +4516,7 @@
       <c r="A4" s="16"/>
       <c r="B4" s="24"/>
       <c r="C4" s="71" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>98</v>
@@ -4349,7 +4538,7 @@
       <c r="A5" s="16"/>
       <c r="B5" s="24"/>
       <c r="C5" s="71" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
@@ -4371,7 +4560,7 @@
       <c r="A6" s="16"/>
       <c r="B6" s="24"/>
       <c r="C6" s="71" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>65</v>
@@ -4393,7 +4582,7 @@
       <c r="A7" s="16"/>
       <c r="B7" s="24"/>
       <c r="C7" s="71" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>99</v>
@@ -4415,7 +4604,7 @@
       <c r="A8" s="16"/>
       <c r="B8" s="24"/>
       <c r="C8" s="71" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>100</v>
@@ -4435,13 +4624,13 @@
       <c r="A9" s="16"/>
       <c r="B9" s="24"/>
       <c r="C9" s="71" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -4453,7 +4642,7 @@
       <c r="A10" s="19"/>
       <c r="B10" s="25"/>
       <c r="C10" s="71" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>23</v>
@@ -4493,7 +4682,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4512,7 +4701,7 @@
         <v>42</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C1" s="32" t="s">
         <v>74</v>
@@ -4524,7 +4713,7 @@
         <v>39</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G1" s="35" t="s">
         <v>40</v>
@@ -4827,10 +5016,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H80"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4877,7 +5066,7 @@
       </c>
       <c r="B2" s="27"/>
       <c r="C2" s="28" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>6</v>
@@ -4898,7 +5087,7 @@
     <row r="3" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="56"/>
       <c r="B3" s="61" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C3" s="62"/>
       <c r="D3" s="45" t="s">
@@ -4976,47 +5165,49 @@
       <c r="H6" s="17"/>
     </row>
     <row r="7" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="26" t="s">
-        <v>257</v>
-      </c>
+      <c r="A7" s="41"/>
       <c r="B7" s="57"/>
       <c r="C7" s="58"/>
       <c r="D7" s="1" t="s">
-        <v>133</v>
+        <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="17"/>
-    </row>
-    <row r="8" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="41"/>
-      <c r="B8" s="57"/>
-      <c r="C8" s="58"/>
+        <v>37</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="H7" s="49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="16"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="3"/>
       <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>148</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="H8" s="49" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="H8" s="17"/>
+    </row>
+    <row r="9" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="24"/>
       <c r="C9" s="3"/>
       <c r="D9" s="1" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>67</v>
@@ -5024,95 +5215,97 @@
       <c r="F9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>139</v>
+      <c r="G9" s="34" t="s">
+        <v>258</v>
       </c>
       <c r="H9" s="17"/>
     </row>
-    <row r="10" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="16"/>
       <c r="B10" s="24"/>
       <c r="C10" s="3"/>
       <c r="D10" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="34" t="s">
-        <v>259</v>
-      </c>
-      <c r="H10" s="17"/>
+      <c r="G10" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="16"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="A11" s="42"/>
+      <c r="B11" s="43" t="s">
+        <v>172</v>
+      </c>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="H11" s="46" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="16"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="H11" s="18"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="42"/>
-      <c r="B12" s="43" t="s">
-        <v>172</v>
-      </c>
-      <c r="C12" s="44"/>
-      <c r="D12" s="45" t="s">
-        <v>141</v>
-      </c>
-      <c r="E12" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="G12" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="H12" s="46" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G12" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="H12" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="24"/>
       <c r="C13" s="3"/>
       <c r="D13" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G13" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="24"/>
       <c r="C14" s="3"/>
       <c r="D14" s="1" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>33</v>
@@ -5121,18 +5314,18 @@
         <v>20</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="24"/>
       <c r="C15" s="3"/>
       <c r="D15" s="1" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>33</v>
@@ -5141,18 +5334,18 @@
         <v>20</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="24"/>
       <c r="C16" s="3"/>
       <c r="D16" s="1" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>33</v>
@@ -5161,79 +5354,77 @@
         <v>20</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="24"/>
       <c r="C17" s="3"/>
       <c r="D17" s="1" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>33</v>
+        <v>163</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G17" s="34" t="s">
-        <v>158</v>
-      </c>
-      <c r="H17" s="18" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="24"/>
       <c r="C18" s="3"/>
       <c r="D18" s="1" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>163</v>
+        <v>67</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>20</v>
+        <v>134</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>161</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>162</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="H18" s="17"/>
     </row>
     <row r="19" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="B19" s="24"/>
       <c r="C19" s="3"/>
       <c r="D19" s="1" t="s">
-        <v>165</v>
+        <v>231</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>67</v>
+        <v>230</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>134</v>
+        <v>20</v>
       </c>
       <c r="G19" s="34" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="H19" s="17"/>
     </row>
-    <row r="20" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="24"/>
       <c r="C20" s="3"/>
       <c r="D20" s="1" t="s">
-        <v>231</v>
+        <v>166</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>230</v>
+        <v>19</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>20</v>
@@ -5243,12 +5434,12 @@
       </c>
       <c r="H20" s="17"/>
     </row>
-    <row r="21" spans="1:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="24"/>
       <c r="C21" s="3"/>
       <c r="D21" s="1" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>19</v>
@@ -5257,66 +5448,68 @@
         <v>20</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H21" s="17"/>
     </row>
-    <row r="22" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="24"/>
       <c r="C22" s="3"/>
       <c r="D22" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="F22" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="H22" s="17"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="42"/>
+      <c r="B23" s="43" t="s">
+        <v>173</v>
+      </c>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45" t="s">
+        <v>174</v>
+      </c>
+      <c r="E23" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="G23" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="H23" s="48" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="16"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G22" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="H22" s="17"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="16"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G23" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="H23" s="17"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="42"/>
-      <c r="B24" s="43" t="s">
-        <v>173</v>
-      </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="E24" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="G24" s="47" t="s">
-        <v>175</v>
-      </c>
-      <c r="H24" s="48" t="s">
-        <v>176</v>
+      <c r="G24" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="H24" s="49" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -5324,27 +5517,25 @@
       <c r="B25" s="24"/>
       <c r="C25" s="3"/>
       <c r="D25" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G25" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="H25" s="49" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+      <c r="H25" s="49"/>
+    </row>
+    <row r="26" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
       <c r="B26" s="24"/>
       <c r="C26" s="3"/>
       <c r="D26" s="1" t="s">
-        <v>178</v>
+        <v>269</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>19</v>
@@ -5355,43 +5546,43 @@
       <c r="G26" s="34" t="s">
         <v>271</v>
       </c>
-      <c r="H26" s="49"/>
-    </row>
-    <row r="27" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H26" s="17" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="24"/>
       <c r="C27" s="3"/>
       <c r="D27" s="1" t="s">
-        <v>270</v>
+        <v>231</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>19</v>
+        <v>230</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>272</v>
-      </c>
-      <c r="H27" s="17" t="s">
-        <v>186</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="H27" s="17"/>
     </row>
     <row r="28" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="24"/>
       <c r="C28" s="3"/>
       <c r="D28" s="1" t="s">
-        <v>231</v>
+        <v>179</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>230</v>
+        <v>19</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>184</v>
+        <v>272</v>
       </c>
       <c r="H28" s="17"/>
     </row>
@@ -5400,7 +5591,7 @@
       <c r="B29" s="24"/>
       <c r="C29" s="3"/>
       <c r="D29" s="1" t="s">
-        <v>179</v>
+        <v>273</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>19</v>
@@ -5409,16 +5600,18 @@
         <v>20</v>
       </c>
       <c r="G29" s="34" t="s">
-        <v>273</v>
-      </c>
-      <c r="H29" s="17"/>
+        <v>274</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="30" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="24"/>
       <c r="C30" s="3"/>
       <c r="D30" s="1" t="s">
-        <v>274</v>
+        <v>180</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>19</v>
@@ -5427,18 +5620,16 @@
         <v>20</v>
       </c>
       <c r="G30" s="34" t="s">
-        <v>275</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+        <v>276</v>
+      </c>
+      <c r="H30" s="17"/>
+    </row>
+    <row r="31" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="24"/>
       <c r="C31" s="3"/>
       <c r="D31" s="1" t="s">
-        <v>180</v>
+        <v>275</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>19</v>
@@ -5449,150 +5640,150 @@
       <c r="G31" s="34" t="s">
         <v>277</v>
       </c>
-      <c r="H31" s="17"/>
-    </row>
-    <row r="32" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H31" s="17" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="24"/>
       <c r="C32" s="3"/>
       <c r="D32" s="1" t="s">
-        <v>276</v>
+        <v>181</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>278</v>
+        <v>185</v>
       </c>
       <c r="H32" s="17" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="24"/>
       <c r="C33" s="3"/>
       <c r="D33" s="1" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="F33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G33" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="H33" s="17"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="42"/>
+      <c r="B34" s="43" t="s">
+        <v>188</v>
+      </c>
+      <c r="C34" s="44"/>
+      <c r="D34" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="E34" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F34" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="H34" s="48" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="51"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="54" t="s">
+        <v>191</v>
+      </c>
+      <c r="E35" s="54" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="54" t="s">
         <v>20</v>
       </c>
-      <c r="G33" s="34" t="s">
-        <v>185</v>
-      </c>
-      <c r="H33" s="17" t="s">
+      <c r="G35" s="55" t="s">
+        <v>283</v>
+      </c>
+      <c r="H35" s="60"/>
+    </row>
+    <row r="36" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="16"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G36" s="34" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G34" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="H34" s="17"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="42"/>
-      <c r="B35" s="43" t="s">
-        <v>188</v>
-      </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="E35" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="F35" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="G35" s="47" t="s">
-        <v>175</v>
-      </c>
-      <c r="H35" s="48" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="51"/>
-      <c r="B36" s="52"/>
-      <c r="C36" s="53"/>
-      <c r="D36" s="54" t="s">
-        <v>191</v>
-      </c>
-      <c r="E36" s="54" t="s">
-        <v>19</v>
-      </c>
-      <c r="F36" s="54" t="s">
-        <v>20</v>
-      </c>
-      <c r="G36" s="55" t="s">
-        <v>284</v>
-      </c>
-      <c r="H36" s="60"/>
+      <c r="H36" s="17" t="s">
+        <v>232</v>
+      </c>
     </row>
     <row r="37" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="24"/>
       <c r="C37" s="3"/>
       <c r="D37" s="1" t="s">
-        <v>282</v>
+        <v>231</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>19</v>
+        <v>230</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G37" s="34" t="s">
-        <v>281</v>
-      </c>
-      <c r="H37" s="17" t="s">
-        <v>232</v>
-      </c>
+        <v>234</v>
+      </c>
+      <c r="H37" s="17"/>
     </row>
     <row r="38" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="24"/>
       <c r="C38" s="3"/>
       <c r="D38" s="1" t="s">
-        <v>231</v>
+        <v>192</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>230</v>
+        <v>19</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G38" s="34" t="s">
-        <v>234</v>
+        <v>284</v>
       </c>
       <c r="H38" s="17"/>
     </row>
-    <row r="39" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="24"/>
       <c r="C39" s="3"/>
       <c r="D39" s="1" t="s">
-        <v>192</v>
+        <v>282</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>19</v>
@@ -5601,16 +5792,18 @@
         <v>20</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>285</v>
-      </c>
-      <c r="H39" s="17"/>
+        <v>286</v>
+      </c>
+      <c r="H39" s="17" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="24"/>
       <c r="C40" s="3"/>
       <c r="D40" s="1" t="s">
-        <v>283</v>
+        <v>193</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>19</v>
@@ -5619,18 +5812,16 @@
         <v>20</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>287</v>
-      </c>
-      <c r="H40" s="17" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>285</v>
+      </c>
+      <c r="H40" s="17"/>
+    </row>
+    <row r="41" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="24"/>
       <c r="C41" s="3"/>
       <c r="D41" s="1" t="s">
-        <v>193</v>
+        <v>289</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>19</v>
@@ -5639,28 +5830,30 @@
         <v>20</v>
       </c>
       <c r="G41" s="34" t="s">
-        <v>286</v>
-      </c>
-      <c r="H41" s="17"/>
-    </row>
-    <row r="42" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>287</v>
+      </c>
+      <c r="H41" s="17" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="24"/>
       <c r="C42" s="3"/>
       <c r="D42" s="1" t="s">
-        <v>290</v>
+        <v>197</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G42" s="34" t="s">
-        <v>288</v>
-      </c>
-      <c r="H42" s="17" t="s">
-        <v>289</v>
+        <v>294</v>
+      </c>
+      <c r="H42" s="18" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5668,7 +5861,7 @@
       <c r="B43" s="24"/>
       <c r="C43" s="3"/>
       <c r="D43" s="1" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>33</v>
@@ -5677,10 +5870,10 @@
         <v>20</v>
       </c>
       <c r="G43" s="34" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>299</v>
+        <v>262</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5688,7 +5881,7 @@
       <c r="B44" s="24"/>
       <c r="C44" s="3"/>
       <c r="D44" s="1" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>33</v>
@@ -5697,10 +5890,10 @@
         <v>20</v>
       </c>
       <c r="G44" s="34" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>263</v>
+        <v>299</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5708,7 +5901,7 @@
       <c r="B45" s="24"/>
       <c r="C45" s="3"/>
       <c r="D45" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>33</v>
@@ -5720,27 +5913,27 @@
         <v>296</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="16"/>
       <c r="B46" s="24"/>
       <c r="C46" s="3"/>
       <c r="D46" s="1" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="G46" s="34" t="s">
-        <v>297</v>
-      </c>
-      <c r="H46" s="18" t="s">
-        <v>264</v>
+        <v>235</v>
+      </c>
+      <c r="H46" s="17" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -5748,20 +5941,18 @@
       <c r="B47" s="24"/>
       <c r="C47" s="3"/>
       <c r="D47" s="1" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>13</v>
+        <v>67</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="G47" s="34" t="s">
-        <v>235</v>
-      </c>
-      <c r="H47" s="17" t="s">
-        <v>236</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="H47" s="17"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="16"/>
@@ -5782,223 +5973,225 @@
       <c r="H48" s="17"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A49" s="16"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="1" t="s">
+      <c r="A49" s="42"/>
+      <c r="B49" s="43" t="s">
+        <v>237</v>
+      </c>
+      <c r="C49" s="44"/>
+      <c r="D49" s="45" t="s">
+        <v>200</v>
+      </c>
+      <c r="E49" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F49" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="G49" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="H49" s="48" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="16"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E50" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F49" s="1" t="s">
+      <c r="F50" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G49" s="34" t="s">
+      <c r="G50" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="H49" s="17"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A50" s="42"/>
-      <c r="B50" s="43" t="s">
-        <v>237</v>
-      </c>
-      <c r="C50" s="44"/>
-      <c r="D50" s="45" t="s">
-        <v>200</v>
-      </c>
-      <c r="E50" s="45" t="s">
+      <c r="H50" s="17"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="42"/>
+      <c r="B51" s="43" t="s">
+        <v>201</v>
+      </c>
+      <c r="C51" s="44"/>
+      <c r="D51" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="E51" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="F50" s="45" t="s">
+      <c r="F51" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="G50" s="47" t="s">
+      <c r="G51" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="H50" s="48" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A51" s="16"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="1" t="s">
+      <c r="H51" s="48" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" s="51"/>
+      <c r="B52" s="52"/>
+      <c r="C52" s="53"/>
+      <c r="D52" s="54" t="s">
+        <v>204</v>
+      </c>
+      <c r="E52" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="F52" s="54" t="s">
+        <v>20</v>
+      </c>
+      <c r="G52" s="55" t="s">
+        <v>238</v>
+      </c>
+      <c r="H52" s="59" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="16"/>
+      <c r="B53" s="24"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="E53" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F51" s="1" t="s">
+      <c r="F53" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G51" s="34" t="s">
+      <c r="G53" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="H51" s="17"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A52" s="42"/>
-      <c r="B52" s="43" t="s">
-        <v>201</v>
-      </c>
-      <c r="C52" s="44"/>
-      <c r="D52" s="45" t="s">
-        <v>202</v>
-      </c>
-      <c r="E52" s="45" t="s">
+      <c r="H53" s="17"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="42"/>
+      <c r="B54" s="43" t="s">
+        <v>239</v>
+      </c>
+      <c r="C54" s="44"/>
+      <c r="D54" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="E54" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="F52" s="45" t="s">
+      <c r="F54" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="G52" s="47" t="s">
+      <c r="G54" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="H52" s="48" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="51"/>
-      <c r="B53" s="52"/>
-      <c r="C53" s="53"/>
-      <c r="D53" s="54" t="s">
-        <v>204</v>
-      </c>
-      <c r="E53" s="54" t="s">
-        <v>33</v>
-      </c>
-      <c r="F53" s="54" t="s">
+      <c r="H54" s="48" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="16"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="3"/>
+      <c r="D55" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G55" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="H55" s="17"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="42"/>
+      <c r="B56" s="43" t="s">
+        <v>207</v>
+      </c>
+      <c r="C56" s="44"/>
+      <c r="D56" s="45" t="s">
+        <v>208</v>
+      </c>
+      <c r="E56" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F56" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="G56" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="H56" s="48" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="16"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G57" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="H57" s="17"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="42"/>
+      <c r="B58" s="43" t="s">
+        <v>210</v>
+      </c>
+      <c r="C58" s="44"/>
+      <c r="D58" s="45" t="s">
+        <v>211</v>
+      </c>
+      <c r="E58" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F58" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="G58" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="H58" s="48" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="16"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G53" s="55" t="s">
-        <v>238</v>
-      </c>
-      <c r="H53" s="59" t="s">
+      <c r="G59" s="34" t="s">
+        <v>182</v>
+      </c>
+      <c r="H59" s="17" t="s">
         <v>265</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A54" s="16"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="3"/>
-      <c r="D54" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G54" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="H54" s="17"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A55" s="42"/>
-      <c r="B55" s="43" t="s">
-        <v>239</v>
-      </c>
-      <c r="C55" s="44"/>
-      <c r="D55" s="45" t="s">
-        <v>205</v>
-      </c>
-      <c r="E55" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="F55" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="G55" s="47" t="s">
-        <v>175</v>
-      </c>
-      <c r="H55" s="48" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A56" s="16"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E56" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G56" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="H56" s="17"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A57" s="42"/>
-      <c r="B57" s="43" t="s">
-        <v>207</v>
-      </c>
-      <c r="C57" s="44"/>
-      <c r="D57" s="45" t="s">
-        <v>208</v>
-      </c>
-      <c r="E57" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="F57" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="G57" s="47" t="s">
-        <v>175</v>
-      </c>
-      <c r="H57" s="48" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A58" s="16"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="3"/>
-      <c r="D58" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G58" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="H58" s="17"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A59" s="42"/>
-      <c r="B59" s="43" t="s">
-        <v>210</v>
-      </c>
-      <c r="C59" s="44"/>
-      <c r="D59" s="45" t="s">
-        <v>211</v>
-      </c>
-      <c r="E59" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="F59" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="G59" s="47" t="s">
-        <v>175</v>
-      </c>
-      <c r="H59" s="48" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6006,7 +6199,7 @@
       <c r="B60" s="24"/>
       <c r="C60" s="3"/>
       <c r="D60" s="1" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>13</v>
@@ -6015,56 +6208,56 @@
         <v>20</v>
       </c>
       <c r="G60" s="34" t="s">
-        <v>182</v>
-      </c>
-      <c r="H60" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="H60" s="49" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
       <c r="B61" s="24"/>
       <c r="C61" s="3"/>
       <c r="D61" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G61" s="34" t="s">
-        <v>240</v>
-      </c>
-      <c r="H61" s="49" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+        <v>241</v>
+      </c>
+      <c r="H61" s="17"/>
+    </row>
+    <row r="62" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="16"/>
       <c r="B62" s="24"/>
       <c r="C62" s="3"/>
       <c r="D62" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G62" s="34" t="s">
-        <v>241</v>
-      </c>
-      <c r="H62" s="17"/>
+        <v>242</v>
+      </c>
+      <c r="H62" s="17" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="63" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
       <c r="B63" s="24"/>
       <c r="C63" s="3"/>
       <c r="D63" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>33</v>
@@ -6073,10 +6266,10 @@
         <v>20</v>
       </c>
       <c r="G63" s="34" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="H63" s="17" t="s">
-        <v>268</v>
+        <v>244</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6084,7 +6277,7 @@
       <c r="B64" s="24"/>
       <c r="C64" s="3"/>
       <c r="D64" s="1" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>33</v>
@@ -6093,56 +6286,54 @@
         <v>20</v>
       </c>
       <c r="G64" s="34" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="H64" s="17" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="16"/>
       <c r="B65" s="24"/>
       <c r="C65" s="3"/>
       <c r="D65" s="1" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>33</v>
+        <v>230</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G65" s="34" t="s">
-        <v>245</v>
-      </c>
-      <c r="H65" s="17" t="s">
-        <v>246</v>
-      </c>
+        <v>248</v>
+      </c>
+      <c r="H65" s="17"/>
     </row>
     <row r="66" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16"/>
       <c r="B66" s="24"/>
       <c r="C66" s="3"/>
       <c r="D66" s="1" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>230</v>
+        <v>19</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G66" s="34" t="s">
-        <v>248</v>
+        <v>290</v>
       </c>
       <c r="H66" s="17"/>
     </row>
-    <row r="67" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A67" s="16"/>
       <c r="B67" s="24"/>
       <c r="C67" s="3"/>
       <c r="D67" s="1" t="s">
-        <v>219</v>
+        <v>291</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>19</v>
@@ -6151,16 +6342,18 @@
         <v>20</v>
       </c>
       <c r="G67" s="34" t="s">
-        <v>291</v>
-      </c>
-      <c r="H67" s="17"/>
-    </row>
-    <row r="68" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="H67" s="17" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="16"/>
       <c r="B68" s="24"/>
       <c r="C68" s="3"/>
       <c r="D68" s="1" t="s">
-        <v>292</v>
+        <v>220</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>19</v>
@@ -6169,13 +6362,11 @@
         <v>20</v>
       </c>
       <c r="G68" s="34" t="s">
-        <v>269</v>
-      </c>
-      <c r="H68" s="17" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+        <v>293</v>
+      </c>
+      <c r="H68" s="17"/>
+    </row>
+    <row r="69" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="16"/>
       <c r="B69" s="24"/>
       <c r="C69" s="3"/>
@@ -6189,56 +6380,56 @@
         <v>20</v>
       </c>
       <c r="G69" s="34" t="s">
-        <v>294</v>
-      </c>
-      <c r="H69" s="17"/>
-    </row>
-    <row r="70" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>292</v>
+      </c>
+      <c r="H69" s="17" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70" s="16"/>
       <c r="B70" s="24"/>
       <c r="C70" s="3"/>
       <c r="D70" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="G70" s="34" t="s">
-        <v>293</v>
+        <v>235</v>
       </c>
       <c r="H70" s="17" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="16"/>
       <c r="B71" s="24"/>
       <c r="C71" s="3"/>
       <c r="D71" s="1" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="G71" s="34" t="s">
-        <v>235</v>
-      </c>
-      <c r="H71" s="17" t="s">
-        <v>250</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="H71" s="17"/>
     </row>
     <row r="72" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="16"/>
       <c r="B72" s="24"/>
       <c r="C72" s="3"/>
       <c r="D72" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>19</v>
@@ -6247,153 +6438,135 @@
         <v>20</v>
       </c>
       <c r="G72" s="34" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="H72" s="17"/>
     </row>
-    <row r="73" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="16"/>
       <c r="B73" s="24"/>
       <c r="C73" s="3"/>
       <c r="D73" s="1" t="s">
-        <v>223</v>
+        <v>171</v>
       </c>
       <c r="E73" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G73" s="34" t="s">
+        <v>170</v>
+      </c>
+      <c r="H73" s="17"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" s="42"/>
+      <c r="B74" s="43" t="s">
+        <v>224</v>
+      </c>
+      <c r="C74" s="44"/>
+      <c r="D74" s="45" t="s">
+        <v>225</v>
+      </c>
+      <c r="E74" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="F74" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="G74" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="H74" s="48" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A75" s="16"/>
+      <c r="B75" s="24"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="E75" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F73" s="1" t="s">
+      <c r="F75" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G73" s="34" t="s">
-        <v>252</v>
-      </c>
-      <c r="H73" s="17"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A74" s="16"/>
-      <c r="B74" s="24"/>
-      <c r="C74" s="3"/>
-      <c r="D74" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G74" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="H74" s="17"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A75" s="42"/>
-      <c r="B75" s="43" t="s">
-        <v>224</v>
-      </c>
-      <c r="C75" s="44"/>
-      <c r="D75" s="45" t="s">
-        <v>225</v>
-      </c>
-      <c r="E75" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="F75" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="G75" s="47" t="s">
-        <v>175</v>
-      </c>
-      <c r="H75" s="48" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A76" s="16"/>
+      <c r="G75" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="H75" s="17"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" s="41"/>
       <c r="B76" s="24"/>
       <c r="C76" s="3"/>
       <c r="D76" s="1" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G76" s="34" t="s">
-        <v>253</v>
+        <v>101</v>
+      </c>
+      <c r="G76" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="H76" s="17"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A77" s="41"/>
+      <c r="A77" s="26" t="s">
+        <v>257</v>
+      </c>
       <c r="B77" s="24"/>
       <c r="C77" s="3"/>
       <c r="D77" s="1" t="s">
-        <v>228</v>
+        <v>133</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G77" s="1" t="s">
-        <v>170</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
       <c r="H77" s="17"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A78" s="26" t="s">
-        <v>258</v>
-      </c>
-      <c r="B78" s="24"/>
-      <c r="C78" s="3"/>
-      <c r="D78" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="17"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A79" s="56"/>
-      <c r="B79" s="43"/>
-      <c r="C79" s="44"/>
-      <c r="D79" s="45" t="s">
+      <c r="A78" s="56"/>
+      <c r="B78" s="43"/>
+      <c r="C78" s="44"/>
+      <c r="D78" s="45" t="s">
         <v>229</v>
       </c>
-      <c r="E79" s="45" t="s">
+      <c r="E78" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="F79" s="45" t="s">
+      <c r="F78" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="G79" s="45" t="s">
+      <c r="G78" s="45" t="s">
         <v>254</v>
       </c>
-      <c r="H79" s="48" t="s">
+      <c r="H78" s="48" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="19"/>
-      <c r="B80" s="25"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="21" t="s">
+    <row r="79" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="19"/>
+      <c r="B79" s="25"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="E80" s="21" t="s">
+      <c r="E79" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F80" s="21"/>
-      <c r="G80" s="21"/>
-      <c r="H80" s="22"/>
+      <c r="F79" s="21"/>
+      <c r="G79" s="21"/>
+      <c r="H79" s="22"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6414,7 +6587,7 @@
           <x14:formula1>
             <xm:f>Keywords!$B:$B</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E80</xm:sqref>
+          <xm:sqref>E1:E79</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
update data and class ExecutionEngine
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -19,7 +19,7 @@
     <sheet name="SignUpPageOriginal" sheetId="2" state="hidden" r:id="rId5"/>
     <sheet name="SignUpPage" sheetId="10" r:id="rId6"/>
     <sheet name="DataOfSignUp" sheetId="5" r:id="rId7"/>
-    <sheet name="CreateCV" sheetId="6" r:id="rId8"/>
+    <sheet name="CreateCV" sheetId="6" state="hidden" r:id="rId8"/>
     <sheet name="DataOfCreateCV" sheetId="7" state="hidden" r:id="rId9"/>
     <sheet name="Search" sheetId="8" state="hidden" r:id="rId10"/>
   </sheets>
@@ -155,9 +155,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Result</t>
-  </si>
-  <si>
     <t xml:space="preserve">        </t>
   </si>
   <si>
@@ -1143,6 +1140,9 @@
   </si>
   <si>
     <t>Validate data in Password field</t>
+  </si>
+  <si>
+    <t>Expected</t>
   </si>
 </sst>
 </file>
@@ -2058,7 +2058,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2082,7 +2082,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2090,7 +2090,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2146,7 +2146,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -2154,7 +2154,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -2162,7 +2162,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2170,7 +2170,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -2178,7 +2178,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -2186,7 +2186,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -2194,7 +2194,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -2202,7 +2202,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -2210,7 +2210,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -2218,7 +2218,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -2226,7 +2226,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -2291,13 +2291,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>0</v>
@@ -2317,11 +2317,11 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B2" s="27"/>
       <c r="C2" s="28" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>6</v>
@@ -2344,7 +2344,7 @@
       <c r="B3" s="24"/>
       <c r="C3" s="3"/>
       <c r="D3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -2356,7 +2356,7 @@
         <v>8</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -2364,7 +2364,7 @@
       <c r="B4" s="24"/>
       <c r="C4" s="3"/>
       <c r="D4" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
@@ -2373,10 +2373,10 @@
         <v>20</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H4" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -2384,7 +2384,7 @@
       <c r="B5" s="24"/>
       <c r="C5" s="3"/>
       <c r="D5" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>19</v>
@@ -2393,7 +2393,7 @@
         <v>20</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="H5" s="18"/>
     </row>
@@ -2402,7 +2402,7 @@
       <c r="B6" s="24"/>
       <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>33</v>
@@ -2411,10 +2411,10 @@
         <v>20</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -2422,7 +2422,7 @@
       <c r="B7" s="24"/>
       <c r="C7" s="3"/>
       <c r="D7" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>33</v>
@@ -2431,10 +2431,10 @@
         <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>310</v>
-      </c>
-      <c r="H7" s="18" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -2442,30 +2442,30 @@
       <c r="B8" s="24"/>
       <c r="C8" s="3"/>
       <c r="D8" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="3"/>
       <c r="D9" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -2479,12 +2479,12 @@
         <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2492,7 +2492,7 @@
       <c r="B11" s="64"/>
       <c r="C11" s="65"/>
       <c r="D11" s="66" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E11" s="66" t="s">
         <v>19</v>
@@ -2501,7 +2501,7 @@
         <v>20</v>
       </c>
       <c r="G11" s="68" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H11" s="67"/>
     </row>
@@ -2510,15 +2510,15 @@
       <c r="B12" s="64"/>
       <c r="C12" s="65"/>
       <c r="D12" s="66" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E12" s="66" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F12" s="66"/>
       <c r="G12" s="66"/>
       <c r="H12" s="67" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
@@ -2526,7 +2526,7 @@
       <c r="B13" s="64"/>
       <c r="C13" s="65"/>
       <c r="D13" s="66" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E13" s="66" t="s">
         <v>37</v>
@@ -2535,10 +2535,10 @@
         <v>20</v>
       </c>
       <c r="G13" s="66" t="s">
+        <v>329</v>
+      </c>
+      <c r="H13" s="67" t="s">
         <v>330</v>
-      </c>
-      <c r="H13" s="67" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -2546,7 +2546,7 @@
       <c r="B14" s="64"/>
       <c r="C14" s="65"/>
       <c r="D14" s="66" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="E14" s="66" t="s">
         <v>37</v>
@@ -2555,10 +2555,10 @@
         <v>20</v>
       </c>
       <c r="G14" s="66" t="s">
+        <v>321</v>
+      </c>
+      <c r="H14" s="69" t="s">
         <v>322</v>
-      </c>
-      <c r="H14" s="69" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -2566,7 +2566,7 @@
       <c r="B15" s="64"/>
       <c r="C15" s="65"/>
       <c r="D15" s="66" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E15" s="66" t="s">
         <v>37</v>
@@ -2575,10 +2575,10 @@
         <v>20</v>
       </c>
       <c r="G15" s="66" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H15" s="67" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -2586,7 +2586,7 @@
       <c r="B16" s="64"/>
       <c r="C16" s="65"/>
       <c r="D16" s="66" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>37</v>
@@ -2595,23 +2595,23 @@
         <v>20</v>
       </c>
       <c r="G16" s="66" t="s">
+        <v>327</v>
+      </c>
+      <c r="H16" s="67" t="s">
         <v>328</v>
-      </c>
-      <c r="H16" s="67" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="26" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B17" s="64"/>
       <c r="C17" s="65"/>
       <c r="D17" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F17" s="66"/>
       <c r="G17" s="66"/>
@@ -2673,7 +2673,7 @@
         <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2689,7 +2689,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2713,7 +2713,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -2721,7 +2721,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2729,7 +2729,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2737,7 +2737,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2745,7 +2745,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2758,7 +2758,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2776,13 +2776,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" s="77" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="C1" s="77" t="s">
         <v>346</v>
-      </c>
-      <c r="C1" s="77" t="s">
-        <v>347</v>
       </c>
       <c r="D1" s="77" t="s">
         <v>0</v>
@@ -2791,24 +2791,24 @@
         <v>26</v>
       </c>
       <c r="F1" s="77" t="s">
+        <v>338</v>
+      </c>
+      <c r="G1" s="77" t="s">
         <v>339</v>
       </c>
-      <c r="G1" s="77" t="s">
-        <v>340</v>
-      </c>
       <c r="H1" s="77" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="75" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="71" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B2" s="78" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D2" s="72" t="s">
         <v>6</v>
@@ -2828,14 +2828,14 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="71" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="71" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -2852,11 +2852,11 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="71" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="71" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
@@ -2874,14 +2874,14 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="71" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="71" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>13</v>
@@ -2898,17 +2898,17 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="71" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="71" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>20</v>
@@ -2920,31 +2920,31 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="71" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="71" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
-      <c r="H7" s="1" t="s">
-        <v>361</v>
+      <c r="H7" s="37" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="71" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="71" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>23</v>
@@ -2958,13 +2958,13 @@
     </row>
     <row r="9" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="71" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B9" s="78" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C9" s="71" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D9" s="72" t="s">
         <v>6</v>
@@ -2984,14 +2984,14 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="71" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="71" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
@@ -3008,11 +3008,11 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="71" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="71" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>12</v>
@@ -3032,14 +3032,14 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="71" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="71" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>13</v>
@@ -3054,17 +3054,17 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="71" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="71" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>20</v>
@@ -3076,31 +3076,31 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="71" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="71" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="71" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="71" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>23</v>
@@ -3156,10 +3156,10 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C1" s="32" t="s">
         <v>38</v>
@@ -3167,42 +3167,42 @@
       <c r="D1" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="32" t="s">
-        <v>40</v>
+      <c r="E1" s="35" t="s">
+        <v>369</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>357</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="E2" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D3" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>360</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -3231,13 +3231,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>0</v>
@@ -3257,10 +3257,10 @@
     </row>
     <row r="2" spans="1:8" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C2" s="28" t="s">
         <v>5</v>
@@ -3286,7 +3286,7 @@
       <c r="B3" s="24"/>
       <c r="C3" s="3"/>
       <c r="D3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -3298,7 +3298,7 @@
         <v>8</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -3306,19 +3306,19 @@
       <c r="B4" s="24"/>
       <c r="C4" s="3"/>
       <c r="D4" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="H4" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -3332,13 +3332,13 @@
         <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -3346,19 +3346,19 @@
       <c r="B6" s="24"/>
       <c r="C6" s="3"/>
       <c r="D6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -3366,19 +3366,19 @@
       <c r="B7" s="24"/>
       <c r="C7" s="3"/>
       <c r="D7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -3386,30 +3386,30 @@
       <c r="B8" s="24"/>
       <c r="C8" s="3"/>
       <c r="D8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H8" s="17"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="26" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="3"/>
       <c r="D9" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -3423,12 +3423,12 @@
         <v>22</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3447,13 +3447,13 @@
     </row>
     <row r="12" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="29" t="s">
         <v>6</v>
@@ -3476,7 +3476,7 @@
       <c r="B13" s="24"/>
       <c r="C13" s="3"/>
       <c r="D13" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>10</v>
@@ -3488,7 +3488,7 @@
         <v>8</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -3496,19 +3496,19 @@
       <c r="B14" s="24"/>
       <c r="C14" s="3"/>
       <c r="D14" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="H14" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -3522,13 +3522,13 @@
         <v>13</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -3536,19 +3536,19 @@
       <c r="B16" s="24"/>
       <c r="C16" s="3"/>
       <c r="D16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -3556,19 +3556,19 @@
       <c r="B17" s="24"/>
       <c r="C17" s="3"/>
       <c r="D17" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -3576,30 +3576,30 @@
       <c r="B18" s="24"/>
       <c r="C18" s="3"/>
       <c r="D18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H18" s="17"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="26" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B19" s="24"/>
       <c r="C19" s="3"/>
       <c r="D19" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -3613,12 +3613,12 @@
         <v>22</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3637,13 +3637,13 @@
     </row>
     <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D22" s="29" t="s">
         <v>6</v>
@@ -3666,7 +3666,7 @@
       <c r="B23" s="24"/>
       <c r="C23" s="3"/>
       <c r="D23" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>10</v>
@@ -3678,7 +3678,7 @@
         <v>8</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -3686,19 +3686,19 @@
       <c r="B24" s="24"/>
       <c r="C24" s="3"/>
       <c r="D24" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="H24" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -3712,13 +3712,13 @@
         <v>13</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -3726,19 +3726,19 @@
       <c r="B26" s="24"/>
       <c r="C26" s="3"/>
       <c r="D26" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -3746,19 +3746,19 @@
       <c r="B27" s="24"/>
       <c r="C27" s="3"/>
       <c r="D27" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H27" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -3766,30 +3766,30 @@
       <c r="B28" s="24"/>
       <c r="C28" s="3"/>
       <c r="D28" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="G28" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H28" s="17"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B29" s="24"/>
       <c r="C29" s="3"/>
       <c r="D29" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -3803,12 +3803,12 @@
         <v>22</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3827,13 +3827,13 @@
     </row>
     <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C32" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D32" s="29" t="s">
         <v>6</v>
@@ -3856,7 +3856,7 @@
       <c r="B33" s="24"/>
       <c r="C33" s="3"/>
       <c r="D33" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>10</v>
@@ -3868,7 +3868,7 @@
         <v>8</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -3876,19 +3876,19 @@
       <c r="B34" s="24"/>
       <c r="C34" s="3"/>
       <c r="D34" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F34" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G34" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G34" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="H34" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -3902,13 +3902,13 @@
         <v>13</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H35" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -3916,19 +3916,19 @@
       <c r="B36" s="24"/>
       <c r="C36" s="3"/>
       <c r="D36" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H36" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -3936,19 +3936,19 @@
       <c r="B37" s="24"/>
       <c r="C37" s="3"/>
       <c r="D37" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H37" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -3956,30 +3956,30 @@
       <c r="B38" s="24"/>
       <c r="C38" s="3"/>
       <c r="D38" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E38" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="G38" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H38" s="17"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B39" s="24"/>
       <c r="C39" s="3"/>
       <c r="D39" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -3993,12 +3993,12 @@
         <v>22</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4017,13 +4017,13 @@
     </row>
     <row r="42" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="B42" s="27" t="s">
-        <v>120</v>
-      </c>
       <c r="C42" s="28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D42" s="29" t="s">
         <v>6</v>
@@ -4046,7 +4046,7 @@
       <c r="B43" s="24"/>
       <c r="C43" s="3"/>
       <c r="D43" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>10</v>
@@ -4058,7 +4058,7 @@
         <v>8</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
@@ -4066,19 +4066,19 @@
       <c r="B44" s="24"/>
       <c r="C44" s="3"/>
       <c r="D44" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G44" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G44" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="H44" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
@@ -4092,13 +4092,13 @@
         <v>13</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H45" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -4106,19 +4106,19 @@
       <c r="B46" s="24"/>
       <c r="C46" s="3"/>
       <c r="D46" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -4126,19 +4126,19 @@
       <c r="B47" s="24"/>
       <c r="C47" s="3"/>
       <c r="D47" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H47" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
@@ -4146,30 +4146,30 @@
       <c r="B48" s="24"/>
       <c r="C48" s="3"/>
       <c r="D48" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E48" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="G48" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H48" s="17"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="26" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B49" s="24"/>
       <c r="C49" s="3"/>
       <c r="D49" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -4183,12 +4183,12 @@
         <v>22</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4207,13 +4207,13 @@
     </row>
     <row r="52" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A52" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B52" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="B52" s="27" t="s">
-        <v>132</v>
-      </c>
       <c r="C52" s="28" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D52" s="29" t="s">
         <v>6</v>
@@ -4236,7 +4236,7 @@
       <c r="B53" s="24"/>
       <c r="C53" s="3"/>
       <c r="D53" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E53" s="1" t="s">
         <v>10</v>
@@ -4248,7 +4248,7 @@
         <v>8</v>
       </c>
       <c r="H53" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
@@ -4256,19 +4256,19 @@
       <c r="B54" s="24"/>
       <c r="C54" s="3"/>
       <c r="D54" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F54" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G54" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="H54" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
@@ -4282,13 +4282,13 @@
         <v>13</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H55" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
@@ -4296,19 +4296,19 @@
       <c r="B56" s="24"/>
       <c r="C56" s="3"/>
       <c r="D56" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H56" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -4316,19 +4316,19 @@
       <c r="B57" s="24"/>
       <c r="C57" s="3"/>
       <c r="D57" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H57" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
@@ -4336,30 +4336,30 @@
       <c r="B58" s="24"/>
       <c r="C58" s="3"/>
       <c r="D58" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F58" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E58" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="G58" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H58" s="17"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="26" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B59" s="24"/>
       <c r="C59" s="3"/>
       <c r="D59" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -4373,12 +4373,12 @@
         <v>22</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4423,7 +4423,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4440,13 +4440,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="77" t="s">
+        <v>344</v>
+      </c>
+      <c r="B1" s="77" t="s">
         <v>345</v>
       </c>
-      <c r="B1" s="77" t="s">
+      <c r="C1" s="77" t="s">
         <v>346</v>
-      </c>
-      <c r="C1" s="77" t="s">
-        <v>347</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>0</v>
@@ -4455,24 +4455,24 @@
         <v>26</v>
       </c>
       <c r="F1" s="14" t="s">
+        <v>338</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>339</v>
       </c>
-      <c r="G1" s="14" t="s">
-        <v>340</v>
-      </c>
       <c r="H1" s="15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="70" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B2" s="78" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D2" s="72" t="s">
         <v>6</v>
@@ -4494,10 +4494,10 @@
       <c r="A3" s="16"/>
       <c r="B3" s="24"/>
       <c r="C3" s="71" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>10</v>
@@ -4509,36 +4509,36 @@
         <v>8</v>
       </c>
       <c r="H3" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="16"/>
       <c r="B4" s="24"/>
       <c r="C4" s="71" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="H4" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="24"/>
       <c r="C5" s="71" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
@@ -4547,76 +4547,76 @@
         <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H5" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="16"/>
       <c r="B6" s="24"/>
       <c r="C6" s="71" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H6" s="18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="16"/>
       <c r="B7" s="24"/>
       <c r="C7" s="71" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="24"/>
       <c r="C8" s="71" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>101</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H8" s="17"/>
     </row>
@@ -4624,25 +4624,25 @@
       <c r="A9" s="16"/>
       <c r="B9" s="24"/>
       <c r="C9" s="71" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19"/>
       <c r="B10" s="25"/>
       <c r="C10" s="71" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>23</v>
@@ -4682,7 +4682,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4698,13 +4698,13 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C1" s="32" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D1" s="32" t="s">
         <v>38</v>
@@ -4713,21 +4713,21 @@
         <v>39</v>
       </c>
       <c r="F1" s="32" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>40</v>
+        <v>369</v>
       </c>
       <c r="H1" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
@@ -4740,21 +4740,21 @@
         <v>18</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>16</v>
@@ -4766,21 +4766,21 @@
         <v>18</v>
       </c>
       <c r="G3" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="7" t="s">
         <v>77</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>78</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="9" t="s">
@@ -4790,24 +4790,24 @@
         <v>18</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="33" t="s">
         <v>18</v>
@@ -4816,24 +4816,24 @@
         <v>18</v>
       </c>
       <c r="G5" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>18</v>
@@ -4842,24 +4842,24 @@
         <v>18</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="33" t="s">
         <v>18</v>
@@ -4868,24 +4868,24 @@
         <v>18</v>
       </c>
       <c r="G7" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>18</v>
@@ -4894,21 +4894,21 @@
         <v>18</v>
       </c>
       <c r="G8" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>16</v>
@@ -4918,47 +4918,47 @@
         <v>18</v>
       </c>
       <c r="G9" s="38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E10" s="33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="33" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H10" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>95</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>16</v>
@@ -4968,21 +4968,21 @@
       </c>
       <c r="F11" s="33"/>
       <c r="G11" s="37" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="11" t="s">
-        <v>97</v>
-      </c>
       <c r="C12" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D12" s="31" t="s">
         <v>16</v>
@@ -4991,13 +4991,13 @@
         <v>18</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G12" s="39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H12" s="36" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -5036,13 +5036,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>0</v>
@@ -5062,11 +5062,11 @@
     </row>
     <row r="2" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B2" s="27"/>
       <c r="C2" s="28" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D2" s="29" t="s">
         <v>6</v>
@@ -5087,11 +5087,11 @@
     <row r="3" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="56"/>
       <c r="B3" s="61" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C3" s="62"/>
       <c r="D3" s="45" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="45" t="s">
         <v>10</v>
@@ -5131,7 +5131,7 @@
       <c r="B5" s="57"/>
       <c r="C5" s="58"/>
       <c r="D5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>13</v>
@@ -5151,10 +5151,10 @@
       <c r="B6" s="57"/>
       <c r="C6" s="58"/>
       <c r="D6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>20</v>
@@ -5178,10 +5178,10 @@
         <v>20</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H7" s="49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -5189,16 +5189,16 @@
       <c r="B8" s="24"/>
       <c r="C8" s="3"/>
       <c r="D8" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H8" s="17"/>
     </row>
@@ -5207,16 +5207,16 @@
       <c r="B9" s="24"/>
       <c r="C9" s="3"/>
       <c r="D9" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H9" s="17"/>
     </row>
@@ -5225,7 +5225,7 @@
       <c r="B10" s="24"/>
       <c r="C10" s="3"/>
       <c r="D10" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>19</v>
@@ -5234,30 +5234,30 @@
         <v>20</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H10" s="18"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="42"/>
       <c r="B11" s="43" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C11" s="44"/>
       <c r="D11" s="45" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E11" s="45" t="s">
         <v>37</v>
       </c>
       <c r="F11" s="45" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G11" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="H11" s="46" t="s">
         <v>142</v>
-      </c>
-      <c r="H11" s="46" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -5265,7 +5265,7 @@
       <c r="B12" s="24"/>
       <c r="C12" s="3"/>
       <c r="D12" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>13</v>
@@ -5274,10 +5274,10 @@
         <v>20</v>
       </c>
       <c r="G12" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="17" t="s">
         <v>144</v>
-      </c>
-      <c r="H12" s="17" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -5285,7 +5285,7 @@
       <c r="B13" s="24"/>
       <c r="C13" s="3"/>
       <c r="D13" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>33</v>
@@ -5294,10 +5294,10 @@
         <v>20</v>
       </c>
       <c r="G13" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="H13" s="18" t="s">
         <v>151</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -5305,7 +5305,7 @@
       <c r="B14" s="24"/>
       <c r="C14" s="3"/>
       <c r="D14" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>33</v>
@@ -5314,10 +5314,10 @@
         <v>20</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -5325,7 +5325,7 @@
       <c r="B15" s="24"/>
       <c r="C15" s="3"/>
       <c r="D15" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>33</v>
@@ -5334,10 +5334,10 @@
         <v>20</v>
       </c>
       <c r="G15" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -5345,7 +5345,7 @@
       <c r="B16" s="24"/>
       <c r="C16" s="3"/>
       <c r="D16" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>33</v>
@@ -5354,10 +5354,10 @@
         <v>20</v>
       </c>
       <c r="G16" s="34" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5365,19 +5365,19 @@
       <c r="B17" s="24"/>
       <c r="C17" s="3"/>
       <c r="D17" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G17" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="H17" s="17" t="s">
         <v>161</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -5385,16 +5385,16 @@
       <c r="B18" s="24"/>
       <c r="C18" s="3"/>
       <c r="D18" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G18" s="34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H18" s="17"/>
     </row>
@@ -5403,16 +5403,16 @@
       <c r="B19" s="24"/>
       <c r="C19" s="3"/>
       <c r="D19" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G19" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H19" s="17"/>
     </row>
@@ -5421,7 +5421,7 @@
       <c r="B20" s="24"/>
       <c r="C20" s="3"/>
       <c r="D20" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>19</v>
@@ -5430,7 +5430,7 @@
         <v>20</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H20" s="17"/>
     </row>
@@ -5439,7 +5439,7 @@
       <c r="B21" s="24"/>
       <c r="C21" s="3"/>
       <c r="D21" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>19</v>
@@ -5448,7 +5448,7 @@
         <v>20</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="H21" s="17"/>
     </row>
@@ -5457,39 +5457,39 @@
       <c r="B22" s="24"/>
       <c r="C22" s="3"/>
       <c r="D22" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G22" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H22" s="17"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="42"/>
       <c r="B23" s="43" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C23" s="44"/>
       <c r="D23" s="45" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E23" s="45" t="s">
         <v>37</v>
       </c>
       <c r="F23" s="45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G23" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="H23" s="48" t="s">
         <v>175</v>
-      </c>
-      <c r="H23" s="48" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -5497,7 +5497,7 @@
       <c r="B24" s="24"/>
       <c r="C24" s="3"/>
       <c r="D24" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>13</v>
@@ -5506,10 +5506,10 @@
         <v>20</v>
       </c>
       <c r="G24" s="34" t="s">
+        <v>181</v>
+      </c>
+      <c r="H24" s="49" t="s">
         <v>182</v>
-      </c>
-      <c r="H24" s="49" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -5517,7 +5517,7 @@
       <c r="B25" s="24"/>
       <c r="C25" s="3"/>
       <c r="D25" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>19</v>
@@ -5526,7 +5526,7 @@
         <v>20</v>
       </c>
       <c r="G25" s="34" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H25" s="49"/>
     </row>
@@ -5535,7 +5535,7 @@
       <c r="B26" s="24"/>
       <c r="C26" s="3"/>
       <c r="D26" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>19</v>
@@ -5544,10 +5544,10 @@
         <v>20</v>
       </c>
       <c r="G26" s="34" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -5555,16 +5555,16 @@
       <c r="B27" s="24"/>
       <c r="C27" s="3"/>
       <c r="D27" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H27" s="17"/>
     </row>
@@ -5573,7 +5573,7 @@
       <c r="B28" s="24"/>
       <c r="C28" s="3"/>
       <c r="D28" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>19</v>
@@ -5582,7 +5582,7 @@
         <v>20</v>
       </c>
       <c r="G28" s="34" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H28" s="17"/>
     </row>
@@ -5591,7 +5591,7 @@
       <c r="B29" s="24"/>
       <c r="C29" s="3"/>
       <c r="D29" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>19</v>
@@ -5600,10 +5600,10 @@
         <v>20</v>
       </c>
       <c r="G29" s="34" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -5611,7 +5611,7 @@
       <c r="B30" s="24"/>
       <c r="C30" s="3"/>
       <c r="D30" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>19</v>
@@ -5620,7 +5620,7 @@
         <v>20</v>
       </c>
       <c r="G30" s="34" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H30" s="17"/>
     </row>
@@ -5629,7 +5629,7 @@
       <c r="B31" s="24"/>
       <c r="C31" s="3"/>
       <c r="D31" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>19</v>
@@ -5638,10 +5638,10 @@
         <v>20</v>
       </c>
       <c r="G31" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="H31" s="17" t="s">
         <v>277</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5649,7 +5649,7 @@
       <c r="B32" s="24"/>
       <c r="C32" s="3"/>
       <c r="D32" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>13</v>
@@ -5658,10 +5658,10 @@
         <v>20</v>
       </c>
       <c r="G32" s="34" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -5669,39 +5669,39 @@
       <c r="B33" s="24"/>
       <c r="C33" s="3"/>
       <c r="D33" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G33" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H33" s="17"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="42"/>
       <c r="B34" s="43" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C34" s="44"/>
       <c r="D34" s="45" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E34" s="45" t="s">
         <v>37</v>
       </c>
       <c r="F34" s="45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G34" s="47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H34" s="48" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5709,7 +5709,7 @@
       <c r="B35" s="52"/>
       <c r="C35" s="53"/>
       <c r="D35" s="54" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E35" s="54" t="s">
         <v>19</v>
@@ -5718,7 +5718,7 @@
         <v>20</v>
       </c>
       <c r="G35" s="55" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H35" s="60"/>
     </row>
@@ -5727,7 +5727,7 @@
       <c r="B36" s="24"/>
       <c r="C36" s="3"/>
       <c r="D36" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>19</v>
@@ -5736,10 +5736,10 @@
         <v>20</v>
       </c>
       <c r="G36" s="34" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H36" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -5747,16 +5747,16 @@
       <c r="B37" s="24"/>
       <c r="C37" s="3"/>
       <c r="D37" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G37" s="34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H37" s="17"/>
     </row>
@@ -5765,7 +5765,7 @@
       <c r="B38" s="24"/>
       <c r="C38" s="3"/>
       <c r="D38" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>19</v>
@@ -5774,7 +5774,7 @@
         <v>20</v>
       </c>
       <c r="G38" s="34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H38" s="17"/>
     </row>
@@ -5783,7 +5783,7 @@
       <c r="B39" s="24"/>
       <c r="C39" s="3"/>
       <c r="D39" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>19</v>
@@ -5792,10 +5792,10 @@
         <v>20</v>
       </c>
       <c r="G39" s="34" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H39" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -5803,7 +5803,7 @@
       <c r="B40" s="24"/>
       <c r="C40" s="3"/>
       <c r="D40" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>19</v>
@@ -5812,7 +5812,7 @@
         <v>20</v>
       </c>
       <c r="G40" s="34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="H40" s="17"/>
     </row>
@@ -5821,7 +5821,7 @@
       <c r="B41" s="24"/>
       <c r="C41" s="3"/>
       <c r="D41" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>19</v>
@@ -5830,10 +5830,10 @@
         <v>20</v>
       </c>
       <c r="G41" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="H41" s="17" t="s">
         <v>287</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5841,7 +5841,7 @@
       <c r="B42" s="24"/>
       <c r="C42" s="3"/>
       <c r="D42" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>33</v>
@@ -5850,10 +5850,10 @@
         <v>20</v>
       </c>
       <c r="G42" s="34" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5861,7 +5861,7 @@
       <c r="B43" s="24"/>
       <c r="C43" s="3"/>
       <c r="D43" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E43" s="1" t="s">
         <v>33</v>
@@ -5870,10 +5870,10 @@
         <v>20</v>
       </c>
       <c r="G43" s="34" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5881,7 +5881,7 @@
       <c r="B44" s="24"/>
       <c r="C44" s="3"/>
       <c r="D44" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>33</v>
@@ -5890,10 +5890,10 @@
         <v>20</v>
       </c>
       <c r="G44" s="34" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -5901,7 +5901,7 @@
       <c r="B45" s="24"/>
       <c r="C45" s="3"/>
       <c r="D45" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>33</v>
@@ -5910,10 +5910,10 @@
         <v>20</v>
       </c>
       <c r="G45" s="34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
@@ -5921,19 +5921,19 @@
       <c r="B46" s="24"/>
       <c r="C46" s="3"/>
       <c r="D46" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G46" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="H46" s="17" t="s">
         <v>235</v>
-      </c>
-      <c r="H46" s="17" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
@@ -5941,16 +5941,16 @@
       <c r="B47" s="24"/>
       <c r="C47" s="3"/>
       <c r="D47" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G47" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H47" s="17"/>
     </row>
@@ -5959,39 +5959,39 @@
       <c r="B48" s="24"/>
       <c r="C48" s="3"/>
       <c r="D48" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G48" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H48" s="17"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="42"/>
       <c r="B49" s="43" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C49" s="44"/>
       <c r="D49" s="45" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E49" s="45" t="s">
         <v>37</v>
       </c>
       <c r="F49" s="45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G49" s="47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H49" s="48" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -5999,39 +5999,39 @@
       <c r="B50" s="24"/>
       <c r="C50" s="3"/>
       <c r="D50" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G50" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H50" s="17"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="42"/>
       <c r="B51" s="43" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C51" s="44"/>
       <c r="D51" s="45" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E51" s="45" t="s">
         <v>37</v>
       </c>
       <c r="F51" s="45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G51" s="47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H51" s="48" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6039,7 +6039,7 @@
       <c r="B52" s="52"/>
       <c r="C52" s="53"/>
       <c r="D52" s="54" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E52" s="54" t="s">
         <v>33</v>
@@ -6048,10 +6048,10 @@
         <v>20</v>
       </c>
       <c r="G52" s="55" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H52" s="59" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
@@ -6059,39 +6059,39 @@
       <c r="B53" s="24"/>
       <c r="C53" s="3"/>
       <c r="D53" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G53" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H53" s="17"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="42"/>
       <c r="B54" s="43" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C54" s="44"/>
       <c r="D54" s="45" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E54" s="45" t="s">
         <v>37</v>
       </c>
       <c r="F54" s="45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G54" s="47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H54" s="48" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
@@ -6099,39 +6099,39 @@
       <c r="B55" s="24"/>
       <c r="C55" s="3"/>
       <c r="D55" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G55" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H55" s="17"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="42"/>
       <c r="B56" s="43" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C56" s="44"/>
       <c r="D56" s="45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E56" s="45" t="s">
         <v>37</v>
       </c>
       <c r="F56" s="45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G56" s="47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H56" s="48" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
@@ -6139,39 +6139,39 @@
       <c r="B57" s="24"/>
       <c r="C57" s="3"/>
       <c r="D57" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G57" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H57" s="17"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="42"/>
       <c r="B58" s="43" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C58" s="44"/>
       <c r="D58" s="45" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E58" s="45" t="s">
         <v>37</v>
       </c>
       <c r="F58" s="45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G58" s="47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H58" s="48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6179,7 +6179,7 @@
       <c r="B59" s="24"/>
       <c r="C59" s="3"/>
       <c r="D59" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>13</v>
@@ -6188,10 +6188,10 @@
         <v>20</v>
       </c>
       <c r="G59" s="34" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H59" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6199,7 +6199,7 @@
       <c r="B60" s="24"/>
       <c r="C60" s="3"/>
       <c r="D60" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>13</v>
@@ -6208,10 +6208,10 @@
         <v>20</v>
       </c>
       <c r="G60" s="34" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H60" s="49" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
@@ -6219,7 +6219,7 @@
       <c r="B61" s="24"/>
       <c r="C61" s="3"/>
       <c r="D61" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>19</v>
@@ -6228,7 +6228,7 @@
         <v>20</v>
       </c>
       <c r="G61" s="34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H61" s="17"/>
     </row>
@@ -6237,7 +6237,7 @@
       <c r="B62" s="24"/>
       <c r="C62" s="3"/>
       <c r="D62" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>33</v>
@@ -6246,10 +6246,10 @@
         <v>20</v>
       </c>
       <c r="G62" s="34" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H62" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6257,7 +6257,7 @@
       <c r="B63" s="24"/>
       <c r="C63" s="3"/>
       <c r="D63" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E63" s="1" t="s">
         <v>33</v>
@@ -6266,10 +6266,10 @@
         <v>20</v>
       </c>
       <c r="G63" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="H63" s="17" t="s">
         <v>243</v>
-      </c>
-      <c r="H63" s="17" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6277,7 +6277,7 @@
       <c r="B64" s="24"/>
       <c r="C64" s="3"/>
       <c r="D64" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>33</v>
@@ -6286,10 +6286,10 @@
         <v>20</v>
       </c>
       <c r="G64" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="H64" s="17" t="s">
         <v>245</v>
-      </c>
-      <c r="H64" s="17" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -6297,16 +6297,16 @@
       <c r="B65" s="24"/>
       <c r="C65" s="3"/>
       <c r="D65" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F65" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G65" s="34" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H65" s="17"/>
     </row>
@@ -6315,7 +6315,7 @@
       <c r="B66" s="24"/>
       <c r="C66" s="3"/>
       <c r="D66" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>19</v>
@@ -6324,7 +6324,7 @@
         <v>20</v>
       </c>
       <c r="G66" s="34" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H66" s="17"/>
     </row>
@@ -6333,7 +6333,7 @@
       <c r="B67" s="24"/>
       <c r="C67" s="3"/>
       <c r="D67" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E67" s="1" t="s">
         <v>19</v>
@@ -6342,10 +6342,10 @@
         <v>20</v>
       </c>
       <c r="G67" s="34" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H67" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6353,7 +6353,7 @@
       <c r="B68" s="24"/>
       <c r="C68" s="3"/>
       <c r="D68" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>19</v>
@@ -6362,7 +6362,7 @@
         <v>20</v>
       </c>
       <c r="G68" s="34" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H68" s="17"/>
     </row>
@@ -6371,7 +6371,7 @@
       <c r="B69" s="24"/>
       <c r="C69" s="3"/>
       <c r="D69" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>19</v>
@@ -6380,10 +6380,10 @@
         <v>20</v>
       </c>
       <c r="G69" s="34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H69" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.3">
@@ -6391,19 +6391,19 @@
       <c r="B70" s="24"/>
       <c r="C70" s="3"/>
       <c r="D70" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E70" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G70" s="34" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H70" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6411,7 +6411,7 @@
       <c r="B71" s="24"/>
       <c r="C71" s="3"/>
       <c r="D71" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E71" s="1" t="s">
         <v>19</v>
@@ -6420,7 +6420,7 @@
         <v>20</v>
       </c>
       <c r="G71" s="34" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H71" s="17"/>
     </row>
@@ -6429,7 +6429,7 @@
       <c r="B72" s="24"/>
       <c r="C72" s="3"/>
       <c r="D72" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>19</v>
@@ -6438,7 +6438,7 @@
         <v>20</v>
       </c>
       <c r="G72" s="34" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H72" s="17"/>
     </row>
@@ -6447,39 +6447,39 @@
       <c r="B73" s="24"/>
       <c r="C73" s="3"/>
       <c r="D73" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G73" s="34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H73" s="17"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="42"/>
       <c r="B74" s="43" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C74" s="44"/>
       <c r="D74" s="45" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E74" s="45" t="s">
         <v>37</v>
       </c>
       <c r="F74" s="45" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G74" s="47" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="H74" s="48" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
@@ -6487,7 +6487,7 @@
       <c r="B75" s="24"/>
       <c r="C75" s="3"/>
       <c r="D75" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E75" s="1" t="s">
         <v>19</v>
@@ -6496,7 +6496,7 @@
         <v>20</v>
       </c>
       <c r="G75" s="34" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H75" s="17"/>
     </row>
@@ -6505,30 +6505,30 @@
       <c r="B76" s="24"/>
       <c r="C76" s="3"/>
       <c r="D76" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H76" s="17"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B77" s="24"/>
       <c r="C77" s="3"/>
       <c r="D77" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -6539,7 +6539,7 @@
       <c r="B78" s="43"/>
       <c r="C78" s="44"/>
       <c r="D78" s="45" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E78" s="45" t="s">
         <v>37</v>
@@ -6548,10 +6548,10 @@
         <v>20</v>
       </c>
       <c r="G78" s="45" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H78" s="48" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
update data from Excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="987" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="371">
   <si>
     <t>Description</t>
   </si>
@@ -1106,9 +1106,6 @@
     <t>SSU_01</t>
   </si>
   <si>
-    <t>20102002</t>
-  </si>
-  <si>
     <t>verifyURL</t>
   </si>
   <si>
@@ -1121,18 +1118,6 @@
     <t>Expected</t>
   </si>
   <si>
-    <t>E-Mail hoặc mật khẩu bị sai. Vui lòng nhập lại</t>
-  </si>
-  <si>
-    <t>Để trống trường Password</t>
-  </si>
-  <si>
-    <t>TC_DN3</t>
-  </si>
-  <si>
-    <t>Nhập sai tài khoản</t>
-  </si>
-  <si>
     <t>Step_1</t>
   </si>
   <si>
@@ -1157,17 +1142,17 @@
     <t>Script_1</t>
   </si>
   <si>
-    <t>TC_DN1</t>
-  </si>
-  <si>
-    <t>TC_DN2</t>
+    <t>SIN_VAL_02</t>
+  </si>
+  <si>
+    <t>SIN_VAL_04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1214,13 +1199,6 @@
       <sz val="11"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF202124"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1520,7 +1498,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1731,7 +1709,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2119,7 +2096,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -2127,7 +2104,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -2839,13 +2816,13 @@
     </row>
     <row r="2" spans="1:8" s="75" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="81" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="B2" s="78" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C2" s="71" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="D2" s="72" t="s">
         <v>6</v>
@@ -2867,7 +2844,7 @@
       <c r="A3" s="80"/>
       <c r="B3" s="3"/>
       <c r="C3" s="71" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>63</v>
@@ -2889,7 +2866,7 @@
       <c r="A4" s="80"/>
       <c r="B4" s="3"/>
       <c r="C4" s="71" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
@@ -2911,7 +2888,7 @@
       <c r="A5" s="80"/>
       <c r="B5" s="3"/>
       <c r="C5" s="71" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>64</v>
@@ -2933,7 +2910,7 @@
       <c r="A6" s="80"/>
       <c r="B6" s="3"/>
       <c r="C6" s="71" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>65</v>
@@ -2953,7 +2930,7 @@
       <c r="A7" s="80"/>
       <c r="B7" s="3"/>
       <c r="C7" s="71" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>22</v>
@@ -2971,7 +2948,7 @@
       <c r="A8" s="80"/>
       <c r="B8" s="3"/>
       <c r="C8" s="71" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>23</v>
@@ -3009,10 +2986,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3039,7 +3016,7 @@
         <v>39</v>
       </c>
       <c r="E1" s="35" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="F1" s="32" t="s">
         <v>56</v>
@@ -3047,51 +3024,48 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>78</v>
       </c>
+      <c r="C2" s="7"/>
       <c r="D2" s="9" t="s">
-        <v>357</v>
-      </c>
-      <c r="E2" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F2" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="37"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>365</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>357</v>
-      </c>
-      <c r="E4" s="82" t="s">
-        <v>362</v>
+        <v>80</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="hoanganh04092001@gmail.com"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4600,7 +4574,7 @@
         <v>342</v>
       </c>
       <c r="G1" s="35" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H1" s="32" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
update data file and ExecutionEngine class
</commit_message>
<xml_diff>
--- a/src/test/resources/data/data.xlsx
+++ b/src/test/resources/data/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9336" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Keywords" sheetId="3" r:id="rId1"/>
@@ -820,39 +820,18 @@
     <t>Step_7</t>
   </si>
   <si>
-    <t>SIN_VAL_02</t>
-  </si>
-  <si>
-    <t>SIN_VAL_04</t>
-  </si>
-  <si>
     <t>varExpected</t>
   </si>
   <si>
     <t>Validate data in text field</t>
   </si>
   <si>
-    <t>ScriptSU</t>
-  </si>
-  <si>
-    <t>ScriptSI</t>
-  </si>
-  <si>
-    <t>SIN_VAL_07</t>
-  </si>
-  <si>
-    <t>SIN_VAL_08</t>
-  </si>
-  <si>
     <t>Nhập thiếu "." trong trường email</t>
   </si>
   <si>
     <t>E-Mail hoặc mật khẩu bị sai. Vui lòng nhập lại</t>
   </si>
   <si>
-    <t>SIN_VAL_12</t>
-  </si>
-  <si>
     <t>//span[contains(text(),'Nguyễn Hoàng Anh')]</t>
   </si>
   <si>
@@ -1126,27 +1105,6 @@
     <t>ScriptCCV</t>
   </si>
   <si>
-    <t>SUP_VAL_02</t>
-  </si>
-  <si>
-    <t>SUP_VAL_08</t>
-  </si>
-  <si>
-    <t>SUP_VAL_10</t>
-  </si>
-  <si>
-    <t>SUP_VAL_14</t>
-  </si>
-  <si>
-    <t>SUP_VAL_18</t>
-  </si>
-  <si>
-    <t>SUP_VAL_21</t>
-  </si>
-  <si>
-    <t>SUP_VAL_22</t>
-  </si>
-  <si>
     <t>Nhập dữ liệu khác dữ liệu trong trường Mật khẩu</t>
   </si>
   <si>
@@ -1205,6 +1163,48 @@
   </si>
   <si>
     <t>Search and view job details</t>
+  </si>
+  <si>
+    <t>SIN_VAL_01</t>
+  </si>
+  <si>
+    <t>SIN_TD_02</t>
+  </si>
+  <si>
+    <t>SIN_TD_04</t>
+  </si>
+  <si>
+    <t>SIN_TD_06</t>
+  </si>
+  <si>
+    <t>SIN_TD_07</t>
+  </si>
+  <si>
+    <t>SIN_TD_11</t>
+  </si>
+  <si>
+    <t>SUP_VAL_01</t>
+  </si>
+  <si>
+    <t>SUP_TD_02</t>
+  </si>
+  <si>
+    <t>SUP_TD_08</t>
+  </si>
+  <si>
+    <t>SUP_TD_10</t>
+  </si>
+  <si>
+    <t>SUP_TD_14</t>
+  </si>
+  <si>
+    <t>SUP_TD_18</t>
+  </si>
+  <si>
+    <t>SUP_TD_19</t>
+  </si>
+  <si>
+    <t>SUP_TD_20</t>
   </si>
 </sst>
 </file>
@@ -2431,7 +2431,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2475,10 +2475,10 @@
     </row>
     <row r="2" spans="1:8" s="53" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="59" t="s">
-        <v>267</v>
+        <v>377</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C2" s="49" t="s">
         <v>255</v>
@@ -2600,7 +2600,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="29" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -2647,8 +2647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="95" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2683,7 +2683,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>262</v>
+        <v>378</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>56</v>
@@ -2701,13 +2701,13 @@
     </row>
     <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>263</v>
+        <v>379</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>57</v>
       </c>
       <c r="C3" s="82" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="D3" s="8" t="s">
         <v>13</v>
@@ -2721,19 +2721,19 @@
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>268</v>
+        <v>380</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>58</v>
       </c>
       <c r="C4" s="82" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E4" s="60" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>38</v>
@@ -2741,33 +2741,33 @@
     </row>
     <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>269</v>
+        <v>381</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="C5" s="82" t="s">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="61" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="F5" s="61" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>272</v>
+        <v>382</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>59</v>
       </c>
       <c r="C6" s="82" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="7" t="s">
@@ -2794,7 +2794,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2837,10 +2837,10 @@
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="48" t="s">
-        <v>266</v>
+        <v>383</v>
       </c>
       <c r="B2" s="56" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C2" s="49" t="s">
         <v>255</v>
@@ -2995,7 +2995,7 @@
       <c r="A9" s="13"/>
       <c r="B9" s="19"/>
       <c r="C9" s="49" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
@@ -3006,14 +3006,14 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="14" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="16"/>
       <c r="B10" s="20"/>
       <c r="C10" s="49" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D10" s="17" t="s">
         <v>18</v>
@@ -3052,8 +3052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D8"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3096,20 +3096,20 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>364</v>
+        <v>384</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>60</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="82" t="s">
-        <v>379</v>
+        <v>365</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="F2" s="26" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="G2" s="29" t="s">
         <v>41</v>
@@ -3120,7 +3120,7 @@
     </row>
     <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>365</v>
+        <v>385</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>56</v>
@@ -3130,10 +3130,10 @@
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="8" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="F3" s="26" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="G3" s="29" t="s">
         <v>41</v>
@@ -3144,7 +3144,7 @@
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>366</v>
+        <v>386</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>57</v>
@@ -3153,13 +3153,13 @@
         <v>55</v>
       </c>
       <c r="D4" s="82" t="s">
-        <v>373</v>
+        <v>359</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="G4" s="30" t="s">
         <v>42</v>
@@ -3170,7 +3170,7 @@
     </row>
     <row r="5" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>367</v>
+        <v>387</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>58</v>
@@ -3179,16 +3179,16 @@
         <v>55</v>
       </c>
       <c r="D5" s="82" t="s">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>38</v>
@@ -3196,7 +3196,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>368</v>
+        <v>388</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>59</v>
@@ -3205,11 +3205,11 @@
         <v>55</v>
       </c>
       <c r="D6" s="82" t="s">
-        <v>380</v>
+        <v>366</v>
       </c>
       <c r="E6" s="26"/>
       <c r="F6" s="26" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="G6" s="30" t="s">
         <v>41</v>
@@ -3220,7 +3220,7 @@
     </row>
     <row r="7" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>369</v>
+        <v>389</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>61</v>
@@ -3229,10 +3229,10 @@
         <v>55</v>
       </c>
       <c r="D7" s="82" t="s">
-        <v>381</v>
+        <v>367</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="F7" s="26"/>
       <c r="G7" s="29" t="s">
@@ -3244,19 +3244,19 @@
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>370</v>
+        <v>390</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>371</v>
+        <v>357</v>
       </c>
       <c r="C8" s="7" t="s">
         <v>55</v>
       </c>
       <c r="D8" s="82" t="s">
-        <v>378</v>
+        <v>364</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>372</v>
+        <v>358</v>
       </c>
       <c r="F8" s="26" t="s">
         <v>35</v>
@@ -3330,7 +3330,7 @@
     </row>
     <row r="2" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="33" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="B2" s="38" t="s">
         <v>220</v>
@@ -3456,7 +3456,7 @@
         <v>15</v>
       </c>
       <c r="G7" s="36" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="H7" s="66" t="s">
         <v>50</v>
@@ -3486,7 +3486,7 @@
       <c r="A9" s="34"/>
       <c r="B9" s="35"/>
       <c r="C9" s="39" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="D9" s="36" t="s">
         <v>87</v>
@@ -3506,7 +3506,7 @@
       <c r="A10" s="34"/>
       <c r="B10" s="35"/>
       <c r="C10" s="39" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D10" s="36" t="s">
         <v>88</v>
@@ -3518,17 +3518,17 @@
         <v>15</v>
       </c>
       <c r="G10" s="36" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="H10" s="40"/>
     </row>
     <row r="11" spans="1:8" s="62" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A11" s="33"/>
       <c r="B11" s="38" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="C11" s="39" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="D11" s="63" t="s">
         <v>79</v>
@@ -3550,7 +3550,7 @@
       <c r="A12" s="34"/>
       <c r="B12" s="35"/>
       <c r="C12" s="39" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="D12" s="36" t="s">
         <v>85</v>
@@ -3572,7 +3572,7 @@
       <c r="A13" s="34"/>
       <c r="B13" s="35"/>
       <c r="C13" s="39" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="D13" s="36" t="s">
         <v>84</v>
@@ -3594,7 +3594,7 @@
       <c r="A14" s="34"/>
       <c r="B14" s="35"/>
       <c r="C14" s="39" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="D14" s="36" t="s">
         <v>91</v>
@@ -3616,7 +3616,7 @@
       <c r="A15" s="34"/>
       <c r="B15" s="35"/>
       <c r="C15" s="39" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D15" s="36" t="s">
         <v>92</v>
@@ -3638,7 +3638,7 @@
       <c r="A16" s="34"/>
       <c r="B16" s="35"/>
       <c r="C16" s="39" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D16" s="36" t="s">
         <v>93</v>
@@ -3660,10 +3660,10 @@
       <c r="A17" s="34"/>
       <c r="B17" s="35"/>
       <c r="C17" s="39" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D17" s="36" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="E17" s="36" t="s">
         <v>14</v>
@@ -3672,7 +3672,7 @@
         <v>15</v>
       </c>
       <c r="G17" s="37" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="H17" s="40"/>
     </row>
@@ -3680,7 +3680,7 @@
       <c r="A18" s="34"/>
       <c r="B18" s="35"/>
       <c r="C18" s="39" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="D18" s="36" t="s">
         <v>98</v>
@@ -3691,14 +3691,14 @@
       <c r="F18" s="36"/>
       <c r="G18" s="37"/>
       <c r="H18" s="41" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="34"/>
       <c r="B19" s="35"/>
       <c r="C19" s="39" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="D19" s="36" t="s">
         <v>100</v>
@@ -3710,7 +3710,7 @@
         <v>15</v>
       </c>
       <c r="G19" s="37" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="H19" s="41"/>
     </row>
@@ -3718,7 +3718,7 @@
       <c r="A20" s="34"/>
       <c r="B20" s="35"/>
       <c r="C20" s="39" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="D20" s="36" t="s">
         <v>158</v>
@@ -3738,7 +3738,7 @@
       <c r="A21" s="34"/>
       <c r="B21" s="35"/>
       <c r="C21" s="39" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="D21" s="36" t="s">
         <v>101</v>
@@ -3758,7 +3758,7 @@
       <c r="A22" s="34"/>
       <c r="B22" s="35"/>
       <c r="C22" s="39" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="D22" s="36" t="s">
         <v>102</v>
@@ -3778,7 +3778,7 @@
       <c r="A23" s="34"/>
       <c r="B23" s="35"/>
       <c r="C23" s="39" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="D23" s="36" t="s">
         <v>106</v>
@@ -3797,10 +3797,10 @@
     <row r="24" spans="1:8" s="62" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A24" s="33"/>
       <c r="B24" s="38" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C24" s="39" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="D24" s="63" t="s">
         <v>107</v>
@@ -3822,7 +3822,7 @@
       <c r="A25" s="34"/>
       <c r="B25" s="35"/>
       <c r="C25" s="39" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="D25" s="36" t="s">
         <v>110</v>
@@ -3844,7 +3844,7 @@
       <c r="A26" s="34"/>
       <c r="B26" s="35"/>
       <c r="C26" s="39" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="D26" s="36" t="s">
         <v>111</v>
@@ -3864,7 +3864,7 @@
       <c r="A27" s="34"/>
       <c r="B27" s="35"/>
       <c r="C27" s="39" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="D27" s="36" t="s">
         <v>189</v>
@@ -3886,7 +3886,7 @@
       <c r="A28" s="34"/>
       <c r="B28" s="35"/>
       <c r="C28" s="39" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="D28" s="36" t="s">
         <v>158</v>
@@ -3906,7 +3906,7 @@
       <c r="A29" s="34"/>
       <c r="B29" s="35"/>
       <c r="C29" s="39" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="D29" s="36" t="s">
         <v>112</v>
@@ -3926,7 +3926,7 @@
       <c r="A30" s="34"/>
       <c r="B30" s="35"/>
       <c r="C30" s="39" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="D30" s="36" t="s">
         <v>193</v>
@@ -3948,7 +3948,7 @@
       <c r="A31" s="34"/>
       <c r="B31" s="35"/>
       <c r="C31" s="39" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="D31" s="36" t="s">
         <v>113</v>
@@ -3968,7 +3968,7 @@
       <c r="A32" s="34"/>
       <c r="B32" s="35"/>
       <c r="C32" s="39" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="D32" s="36" t="s">
         <v>195</v>
@@ -3990,7 +3990,7 @@
       <c r="A33" s="34"/>
       <c r="B33" s="35"/>
       <c r="C33" s="39" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="D33" s="36" t="s">
         <v>114</v>
@@ -4012,7 +4012,7 @@
       <c r="A34" s="34"/>
       <c r="B34" s="35"/>
       <c r="C34" s="39" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="D34" s="36" t="s">
         <v>106</v>
@@ -4031,10 +4031,10 @@
     <row r="35" spans="1:8" s="62" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A35" s="33"/>
       <c r="B35" s="38" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C35" s="39" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="D35" s="63" t="s">
         <v>121</v>
@@ -4056,7 +4056,7 @@
       <c r="A36" s="34"/>
       <c r="B36" s="35"/>
       <c r="C36" s="39" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="D36" s="36" t="s">
         <v>123</v>
@@ -4076,7 +4076,7 @@
       <c r="A37" s="34"/>
       <c r="B37" s="35"/>
       <c r="C37" s="39" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="D37" s="36" t="s">
         <v>201</v>
@@ -4098,7 +4098,7 @@
       <c r="A38" s="34"/>
       <c r="B38" s="35"/>
       <c r="C38" s="39" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="D38" s="36" t="s">
         <v>158</v>
@@ -4118,7 +4118,7 @@
       <c r="A39" s="34"/>
       <c r="B39" s="35"/>
       <c r="C39" s="39" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="D39" s="36" t="s">
         <v>124</v>
@@ -4138,7 +4138,7 @@
       <c r="A40" s="34"/>
       <c r="B40" s="35"/>
       <c r="C40" s="39" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="D40" s="36" t="s">
         <v>202</v>
@@ -4160,7 +4160,7 @@
       <c r="A41" s="34"/>
       <c r="B41" s="35"/>
       <c r="C41" s="39" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="D41" s="36" t="s">
         <v>125</v>
@@ -4180,7 +4180,7 @@
       <c r="A42" s="33"/>
       <c r="B42" s="77"/>
       <c r="C42" s="39" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="D42" s="63" t="s">
         <v>209</v>
@@ -4202,7 +4202,7 @@
       <c r="A43" s="33"/>
       <c r="B43" s="77"/>
       <c r="C43" s="39" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="D43" s="63" t="s">
         <v>129</v>
@@ -4224,7 +4224,7 @@
       <c r="A44" s="33"/>
       <c r="B44" s="77"/>
       <c r="C44" s="39" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="D44" s="63" t="s">
         <v>126</v>
@@ -4246,7 +4246,7 @@
       <c r="A45" s="33"/>
       <c r="B45" s="77"/>
       <c r="C45" s="39" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="D45" s="63" t="s">
         <v>127</v>
@@ -4268,7 +4268,7 @@
       <c r="A46" s="33"/>
       <c r="B46" s="77"/>
       <c r="C46" s="39" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="D46" s="63" t="s">
         <v>128</v>
@@ -4290,7 +4290,7 @@
       <c r="A47" s="33"/>
       <c r="B47" s="77"/>
       <c r="C47" s="39" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="D47" s="63" t="s">
         <v>130</v>
@@ -4312,7 +4312,7 @@
       <c r="A48" s="33"/>
       <c r="B48" s="77"/>
       <c r="C48" s="39" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="D48" s="63" t="s">
         <v>106</v>
@@ -4332,7 +4332,7 @@
       <c r="A49" s="33"/>
       <c r="B49" s="77"/>
       <c r="C49" s="39" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="D49" s="63" t="s">
         <v>106</v>
@@ -4351,10 +4351,10 @@
     <row r="50" spans="1:8" s="62" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50" s="33"/>
       <c r="B50" s="38" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C50" s="39" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="D50" s="63" t="s">
         <v>132</v>
@@ -4376,7 +4376,7 @@
       <c r="A51" s="33"/>
       <c r="B51" s="77"/>
       <c r="C51" s="39" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="D51" s="63" t="s">
         <v>106</v>
@@ -4395,10 +4395,10 @@
     <row r="52" spans="1:8" s="62" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="73"/>
       <c r="B52" s="38" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="C52" s="39" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="D52" s="74" t="s">
         <v>133</v>
@@ -4413,17 +4413,17 @@
         <v>108</v>
       </c>
       <c r="H52" s="76" t="s">
-        <v>377</v>
+        <v>363</v>
       </c>
     </row>
     <row r="53" spans="1:8" s="62" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53" s="39"/>
       <c r="B53" s="39"/>
       <c r="C53" s="39" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="D53" s="63" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="E53" s="63" t="s">
         <v>14</v>
@@ -4432,7 +4432,7 @@
         <v>15</v>
       </c>
       <c r="G53" s="72" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="H53" s="78"/>
     </row>
@@ -4440,7 +4440,7 @@
       <c r="A54" s="77"/>
       <c r="B54" s="77"/>
       <c r="C54" s="39" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="D54" s="63" t="s">
         <v>134</v>
@@ -4452,7 +4452,7 @@
         <v>15</v>
       </c>
       <c r="G54" s="72" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="H54" s="79"/>
     </row>
@@ -4460,7 +4460,7 @@
       <c r="A55" s="33"/>
       <c r="B55" s="77"/>
       <c r="C55" s="39" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="D55" s="63" t="s">
         <v>106</v>
@@ -4479,10 +4479,10 @@
     <row r="56" spans="1:8" s="62" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="33"/>
       <c r="B56" s="38" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="C56" s="39" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="D56" s="63" t="s">
         <v>135</v>
@@ -4504,7 +4504,7 @@
       <c r="A57" s="33"/>
       <c r="B57" s="77"/>
       <c r="C57" s="39" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="D57" s="63" t="s">
         <v>106</v>
@@ -4523,10 +4523,10 @@
     <row r="58" spans="1:8" s="62" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="33"/>
       <c r="B58" s="38" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C58" s="39" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="D58" s="63" t="s">
         <v>137</v>
@@ -4548,7 +4548,7 @@
       <c r="A59" s="33"/>
       <c r="B59" s="77"/>
       <c r="C59" s="39" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="D59" s="63" t="s">
         <v>106</v>
@@ -4567,10 +4567,10 @@
     <row r="60" spans="1:8" s="62" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" s="33"/>
       <c r="B60" s="38" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C60" s="39" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="D60" s="63" t="s">
         <v>139</v>
@@ -4592,7 +4592,7 @@
       <c r="A61" s="34"/>
       <c r="B61" s="35"/>
       <c r="C61" s="39" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D61" s="36" t="s">
         <v>141</v>
@@ -4614,7 +4614,7 @@
       <c r="A62" s="34"/>
       <c r="B62" s="35"/>
       <c r="C62" s="39" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="D62" s="36" t="s">
         <v>142</v>
@@ -4636,7 +4636,7 @@
       <c r="A63" s="34"/>
       <c r="B63" s="35"/>
       <c r="C63" s="39" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="D63" s="36" t="s">
         <v>143</v>
@@ -4656,7 +4656,7 @@
       <c r="A64" s="34"/>
       <c r="B64" s="35"/>
       <c r="C64" s="39" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="D64" s="36" t="s">
         <v>144</v>
@@ -4678,7 +4678,7 @@
       <c r="A65" s="34"/>
       <c r="B65" s="35"/>
       <c r="C65" s="39" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="D65" s="36" t="s">
         <v>145</v>
@@ -4700,7 +4700,7 @@
       <c r="A66" s="34"/>
       <c r="B66" s="35"/>
       <c r="C66" s="39" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="D66" s="36" t="s">
         <v>146</v>
@@ -4722,7 +4722,7 @@
       <c r="A67" s="34"/>
       <c r="B67" s="35"/>
       <c r="C67" s="39" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="D67" s="36" t="s">
         <v>158</v>
@@ -4742,7 +4742,7 @@
       <c r="A68" s="34"/>
       <c r="B68" s="35"/>
       <c r="C68" s="39" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="D68" s="36" t="s">
         <v>147</v>
@@ -4762,7 +4762,7 @@
       <c r="A69" s="33"/>
       <c r="B69" s="77"/>
       <c r="C69" s="39" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="D69" s="63" t="s">
         <v>211</v>
@@ -4784,7 +4784,7 @@
       <c r="A70" s="33"/>
       <c r="B70" s="77"/>
       <c r="C70" s="39" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="D70" s="63" t="s">
         <v>148</v>
@@ -4804,7 +4804,7 @@
       <c r="A71" s="33"/>
       <c r="B71" s="77"/>
       <c r="C71" s="39" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="D71" s="63" t="s">
         <v>148</v>
@@ -4826,7 +4826,7 @@
       <c r="A72" s="33"/>
       <c r="B72" s="77"/>
       <c r="C72" s="39" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="D72" s="63" t="s">
         <v>149</v>
@@ -4848,7 +4848,7 @@
       <c r="A73" s="33"/>
       <c r="B73" s="77"/>
       <c r="C73" s="39" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="D73" s="63" t="s">
         <v>150</v>
@@ -4868,7 +4868,7 @@
       <c r="A74" s="33"/>
       <c r="B74" s="77"/>
       <c r="C74" s="39" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="D74" s="63" t="s">
         <v>151</v>
@@ -4888,7 +4888,7 @@
       <c r="A75" s="33"/>
       <c r="B75" s="77"/>
       <c r="C75" s="39" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="D75" s="63" t="s">
         <v>106</v>
@@ -4907,10 +4907,10 @@
     <row r="76" spans="1:8" s="62" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="33"/>
       <c r="B76" s="38" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="C76" s="39" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="D76" s="63" t="s">
         <v>152</v>
@@ -4932,7 +4932,7 @@
       <c r="A77" s="33"/>
       <c r="B77" s="77"/>
       <c r="C77" s="39" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="D77" s="63" t="s">
         <v>154</v>
@@ -4952,7 +4952,7 @@
       <c r="A78" s="33"/>
       <c r="B78" s="35"/>
       <c r="C78" s="39" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="D78" s="36" t="s">
         <v>155</v>
@@ -4972,7 +4972,7 @@
       <c r="A79" s="33"/>
       <c r="B79" s="35"/>
       <c r="C79" s="39" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="D79" s="36" t="s">
         <v>156</v>
@@ -4994,7 +4994,7 @@
       <c r="A80" s="67"/>
       <c r="B80" s="68"/>
       <c r="C80" s="39" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="D80" s="69" t="s">
         <v>18</v>
@@ -5101,10 +5101,10 @@
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>389</v>
+        <v>375</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>390</v>
+        <v>376</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>255</v>
@@ -5257,7 +5257,7 @@
       <c r="A9" s="13"/>
       <c r="B9" s="19"/>
       <c r="C9" s="22" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>17</v>
@@ -5268,14 +5268,14 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="84" t="s">
-        <v>388</v>
+        <v>374</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="42"/>
       <c r="B10" s="43"/>
       <c r="C10" s="22" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D10" s="44" t="s">
         <v>235</v>
@@ -5287,7 +5287,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="46" t="s">
-        <v>382</v>
+        <v>368</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -5295,7 +5295,7 @@
       <c r="A11" s="42"/>
       <c r="B11" s="43"/>
       <c r="C11" s="22" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="D11" s="44" t="s">
         <v>237</v>
@@ -5306,14 +5306,14 @@
       <c r="F11" s="44"/>
       <c r="G11" s="44"/>
       <c r="H11" s="83" t="s">
-        <v>383</v>
+        <v>369</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="42"/>
       <c r="B12" s="43"/>
       <c r="C12" s="22" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="D12" s="46" t="s">
         <v>242</v>
@@ -5325,7 +5325,7 @@
         <v>15</v>
       </c>
       <c r="G12" s="44" t="s">
-        <v>384</v>
+        <v>370</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>241</v>
@@ -5335,7 +5335,7 @@
       <c r="A13" s="42"/>
       <c r="B13" s="43"/>
       <c r="C13" s="22" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="D13" s="44" t="s">
         <v>238</v>
@@ -5347,17 +5347,17 @@
         <v>75</v>
       </c>
       <c r="G13" s="44" t="s">
-        <v>385</v>
+        <v>371</v>
       </c>
       <c r="H13" s="47" t="s">
-        <v>386</v>
+        <v>372</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="42"/>
       <c r="B14" s="43"/>
       <c r="C14" s="22" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="D14" s="44" t="s">
         <v>239</v>
@@ -5379,7 +5379,7 @@
       <c r="A15" s="42"/>
       <c r="B15" s="43"/>
       <c r="C15" s="22" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="D15" s="44" t="s">
         <v>240</v>
@@ -5391,7 +5391,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="44" t="s">
-        <v>387</v>
+        <v>373</v>
       </c>
       <c r="H15" s="45" t="s">
         <v>187</v>
@@ -5401,7 +5401,7 @@
       <c r="A16" s="16"/>
       <c r="B16" s="20"/>
       <c r="C16" s="22" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="D16" s="17" t="s">
         <v>18</v>

</xml_diff>